<commit_message>
v 5.61 before dev
</commit_message>
<xml_diff>
--- a/src/main/screeps.xlsx
+++ b/src/main/screeps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00prg\Screeps\screeps-kotlin-starter-master\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA496C4-905F-4CD0-9D79-4C034CDEADB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44636B62-95CE-4DBF-9976-7BFB98BF0EA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="10" activeTab="10" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="10" xr2:uid="{E64D4CD0-F693-495E-97B0-F1DF3284CC0F}"/>
   </bookViews>
   <sheets>
     <sheet name="plan expansion" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,6 @@
     <sheet name="Main2" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3172,7 +3171,7 @@
   <dimension ref="J2:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3261,29 +3260,11 @@
       <c r="K6">
         <v>2</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>2</v>
-      </c>
-      <c r="R6">
-        <v>3</v>
-      </c>
-      <c r="S6">
-        <v>4</v>
-      </c>
-      <c r="T6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="10:32" x14ac:dyDescent="0.25">
       <c r="K7">
         <v>3</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
       <c r="AE7">
         <f>15*1000*24*30*AE2*AF5</f>
         <v>354240000</v>
@@ -3293,46 +3274,34 @@
       <c r="K8">
         <v>4</v>
       </c>
-      <c r="O8">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="S8" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="9" spans="10:32" x14ac:dyDescent="0.25">
       <c r="K9">
         <v>5</v>
       </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="Q9" s="29" t="s">
-        <v>256</v>
+      <c r="R9" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="T9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="10:32" x14ac:dyDescent="0.25">
       <c r="K10">
         <v>6</v>
       </c>
-      <c r="O10">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="30" t="s">
-        <v>257</v>
-      </c>
-      <c r="S10" t="s">
-        <v>5</v>
+      <c r="R10" s="29" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="10:32" x14ac:dyDescent="0.25">
       <c r="K11">
         <v>7</v>
       </c>
-      <c r="O11">
+      <c r="R11" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="T11" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>